<commit_message>
Fixing SEM code. Still not working, but is taking in the models.
</commit_message>
<xml_diff>
--- a/overall_missing.xlsx
+++ b/overall_missing.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1170,7 +1170,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>school2</t>
+          <t>school2_type</t>
         </is>
       </c>
       <c r="B63">
@@ -1183,7 +1183,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>school2_4yr</t>
+          <t>sexual</t>
         </is>
       </c>
       <c r="B64">
@@ -1196,7 +1196,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>school2_ad</t>
+          <t>sib_freq</t>
         </is>
       </c>
       <c r="B65">
@@ -1209,7 +1209,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>school2_cc</t>
+          <t>stig_pcv_2</t>
         </is>
       </c>
       <c r="B66">
@@ -1222,7 +1222,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>sexual</t>
+          <t>stig_pcv_3</t>
         </is>
       </c>
       <c r="B67">
@@ -1235,7 +1235,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>sib_freq</t>
+          <t>talk</t>
         </is>
       </c>
       <c r="B68">
@@ -1248,7 +1248,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>stig_pcv_2</t>
+          <t>ther_vis</t>
         </is>
       </c>
       <c r="B69">
@@ -1261,7 +1261,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>stig_pcv_3</t>
+          <t>wcs_tot</t>
         </is>
       </c>
       <c r="B70">
@@ -1269,45 +1269,6 @@
       </c>
       <c r="C70">
         <v>0.7957243615017304</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>talk</t>
-        </is>
-      </c>
-      <c r="B71">
-        <v>34479</v>
-      </c>
-      <c r="C71">
-        <v>0.7552240767512156</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>ther_vis</t>
-        </is>
-      </c>
-      <c r="B72">
-        <v>35670</v>
-      </c>
-      <c r="C72">
-        <v>0.78131160467867</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>wcs_tot</t>
-        </is>
-      </c>
-      <c r="B73">
-        <v>36352</v>
-      </c>
-      <c r="C73">
-        <v>0.7962500547597143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running right before SEM test run
</commit_message>
<xml_diff>
--- a/overall_missing.xlsx
+++ b/overall_missing.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,7 +390,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>aca_impa</t>
+          <t>abuse_year</t>
         </is>
       </c>
       <c r="B3">
@@ -403,7 +403,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>achieve4</t>
+          <t>aca_impa</t>
         </is>
       </c>
       <c r="B4">
@@ -416,7 +416,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>activ_yn</t>
         </is>
       </c>
       <c r="B5">
@@ -429,7 +429,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>alc_tx</t>
+          <t>age</t>
         </is>
       </c>
       <c r="B6">
@@ -442,7 +442,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>anx_score</t>
+          <t>anx_mod</t>
         </is>
       </c>
       <c r="B7">
@@ -455,7 +455,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>assault_emo</t>
+          <t>anx_sev</t>
         </is>
       </c>
       <c r="B8">
@@ -468,7 +468,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>assault_phys</t>
+          <t>assault_emo</t>
         </is>
       </c>
       <c r="B9">
@@ -481,7 +481,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>assault_sex</t>
+          <t>assault_phys</t>
         </is>
       </c>
       <c r="B10">
@@ -494,7 +494,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>audit_tot</t>
+          <t>assault_sex</t>
         </is>
       </c>
       <c r="B11">
@@ -507,7 +507,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>belong1</t>
+          <t>audit_tot</t>
         </is>
       </c>
       <c r="B12">
@@ -520,7 +520,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>belong2</t>
+          <t>belong1</t>
         </is>
       </c>
       <c r="B13">
@@ -533,7 +533,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>belong8</t>
+          <t>belong2</t>
         </is>
       </c>
       <c r="B14">
@@ -546,7 +546,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>belong9</t>
+          <t>belong8</t>
         </is>
       </c>
       <c r="B15">
@@ -559,7 +559,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>binge_fr</t>
+          <t>belong9</t>
         </is>
       </c>
       <c r="B16">
@@ -572,7 +572,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>body_sr</t>
+          <t>binge_fr</t>
         </is>
       </c>
       <c r="B17">
@@ -585,7 +585,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BRS_tot</t>
+          <t>body_sr</t>
         </is>
       </c>
       <c r="B18">
@@ -598,7 +598,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>dep_impa</t>
+          <t>BRS_tot</t>
         </is>
       </c>
       <c r="B19">
@@ -611,7 +611,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>dep_secret</t>
+          <t>dep_impa</t>
         </is>
       </c>
       <c r="B20">
@@ -624,7 +624,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>deprawsc</t>
+          <t>dep_mod</t>
         </is>
       </c>
       <c r="B21">
@@ -637,7 +637,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>disab_1</t>
+          <t>dep_secret</t>
         </is>
       </c>
       <c r="B22">
@@ -650,7 +650,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>discrim</t>
+          <t>dep_sev</t>
         </is>
       </c>
       <c r="B23">
@@ -663,7 +663,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>divers</t>
+          <t>discrim</t>
         </is>
       </c>
       <c r="B24">
@@ -676,7 +676,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>drug_none</t>
+          <t>divers</t>
         </is>
       </c>
       <c r="B25">
@@ -689,7 +689,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>drug_type</t>
+          <t>drugs_yn</t>
         </is>
       </c>
       <c r="B26">
@@ -741,7 +741,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>dx_ea</t>
+          <t>dx_pers</t>
         </is>
       </c>
       <c r="B30">
@@ -754,7 +754,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>dx_none</t>
+          <t>dx_tr</t>
         </is>
       </c>
       <c r="B31">
@@ -767,7 +767,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>dx_pers</t>
+          <t>ed_any</t>
         </is>
       </c>
       <c r="B32">
@@ -780,7 +780,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>dx_psy</t>
+          <t>env_mh</t>
         </is>
       </c>
       <c r="B33">
@@ -793,7 +793,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>dx_sa</t>
+          <t>fincur</t>
         </is>
       </c>
       <c r="B34">
@@ -806,7 +806,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>dx_tr</t>
+          <t>finpast</t>
         </is>
       </c>
       <c r="B35">
@@ -819,7 +819,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ed_scoff</t>
+          <t>flourish</t>
         </is>
       </c>
       <c r="B36">
@@ -832,7 +832,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>env_mh</t>
+          <t>gad7_impa</t>
         </is>
       </c>
       <c r="B37">
@@ -845,7 +845,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>fam_support_aca</t>
+          <t>gender_noncis</t>
         </is>
       </c>
       <c r="B38">
@@ -858,7 +858,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>fincur</t>
+          <t>gpa_sr</t>
         </is>
       </c>
       <c r="B39">
@@ -871,7 +871,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>finpast</t>
+          <t>inf</t>
         </is>
       </c>
       <c r="B40">
@@ -884,7 +884,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>flourish</t>
+          <t>ins_cover</t>
         </is>
       </c>
       <c r="B41">
@@ -897,7 +897,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>gad7_impa</t>
+          <t>international</t>
         </is>
       </c>
       <c r="B42">
@@ -910,7 +910,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>gender</t>
+          <t>meds_anx</t>
         </is>
       </c>
       <c r="B43">
@@ -923,7 +923,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>gpa_sr</t>
+          <t>meds_count</t>
         </is>
       </c>
       <c r="B44">
@@ -936,7 +936,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>inf</t>
+          <t>meds_dep</t>
         </is>
       </c>
       <c r="B45">
@@ -949,7 +949,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ins_cover</t>
+          <t>meds_mood</t>
         </is>
       </c>
       <c r="B46">
@@ -962,7 +962,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>meds_anx</t>
+          <t>meds_sle</t>
         </is>
       </c>
       <c r="B47">
@@ -975,7 +975,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>meds_count</t>
+          <t>meds_sti</t>
         </is>
       </c>
       <c r="B48">
@@ -988,7 +988,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>meds_dep</t>
+          <t>military</t>
         </is>
       </c>
       <c r="B49">
@@ -1001,7 +1001,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>meds_mood</t>
+          <t>percneed_cur</t>
         </is>
       </c>
       <c r="B50">
@@ -1014,7 +1014,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>meds_none</t>
+          <t>persist</t>
         </is>
       </c>
       <c r="B51">
@@ -1027,7 +1027,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>meds_oth</t>
+          <t>psyhx</t>
         </is>
       </c>
       <c r="B52">
@@ -1040,7 +1040,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>meds_psy</t>
+          <t>race</t>
         </is>
       </c>
       <c r="B53">
@@ -1053,7 +1053,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>meds_sle</t>
+          <t>religios</t>
         </is>
       </c>
       <c r="B54">
@@ -1066,7 +1066,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>meds_sti</t>
+          <t>residenc</t>
         </is>
       </c>
       <c r="B55">
@@ -1079,7 +1079,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>percneed_cur</t>
+          <t>satisfied_overall</t>
         </is>
       </c>
       <c r="B56">
@@ -1092,7 +1092,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>persist</t>
+          <t>school2_type</t>
         </is>
       </c>
       <c r="B57">
@@ -1105,7 +1105,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>psyhx</t>
+          <t>sexual</t>
         </is>
       </c>
       <c r="B58">
@@ -1118,7 +1118,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>race</t>
+          <t>sib_freq</t>
         </is>
       </c>
       <c r="B59">
@@ -1131,7 +1131,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>religios</t>
+          <t>stig_pcv_2</t>
         </is>
       </c>
       <c r="B60">
@@ -1144,7 +1144,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>residenc</t>
+          <t>stig_pcv_3</t>
         </is>
       </c>
       <c r="B61">
@@ -1157,7 +1157,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>satisfied_overall</t>
+          <t>talk</t>
         </is>
       </c>
       <c r="B62">
@@ -1170,7 +1170,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>school2_type</t>
+          <t>ther_vis</t>
         </is>
       </c>
       <c r="B63">
@@ -1178,97 +1178,6 @@
       </c>
       <c r="C63">
         <v>0.7935120690410479</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>sexual</t>
-        </is>
-      </c>
-      <c r="B64">
-        <v>36303</v>
-      </c>
-      <c r="C64">
-        <v>0.7951767643579971</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>sib_freq</t>
-        </is>
-      </c>
-      <c r="B65">
-        <v>36267</v>
-      </c>
-      <c r="C65">
-        <v>0.7943882244710212</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>stig_pcv_2</t>
-        </is>
-      </c>
-      <c r="B66">
-        <v>36182</v>
-      </c>
-      <c r="C66">
-        <v>0.792526394182328</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>stig_pcv_3</t>
-        </is>
-      </c>
-      <c r="B67">
-        <v>36303</v>
-      </c>
-      <c r="C67">
-        <v>0.7951767643579971</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>talk</t>
-        </is>
-      </c>
-      <c r="B68">
-        <v>36314</v>
-      </c>
-      <c r="C68">
-        <v>0.7954177071012397</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>ther_vis</t>
-        </is>
-      </c>
-      <c r="B69">
-        <v>36337</v>
-      </c>
-      <c r="C69">
-        <v>0.7959214964734744</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>wcs_tot</t>
-        </is>
-      </c>
-      <c r="B70">
-        <v>36328</v>
-      </c>
-      <c r="C70">
-        <v>0.7957243615017304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all var summary stats running
</commit_message>
<xml_diff>
--- a/overall_missing.xlsx
+++ b/overall_missing.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,7 +624,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>dep_mod</t>
+          <t>dep_secret</t>
         </is>
       </c>
       <c r="B21">
@@ -637,7 +637,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>dep_secret</t>
+          <t>deprawsc</t>
         </is>
       </c>
       <c r="B22">
@@ -650,7 +650,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>dep_sev</t>
+          <t>discrim</t>
         </is>
       </c>
       <c r="B23">
@@ -663,7 +663,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>discrim</t>
+          <t>divers</t>
         </is>
       </c>
       <c r="B24">
@@ -676,7 +676,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>divers</t>
+          <t>drug_mar</t>
         </is>
       </c>
       <c r="B25">
@@ -689,7 +689,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>drug_mar</t>
+          <t>drugs_yn</t>
         </is>
       </c>
       <c r="B26">
@@ -702,7 +702,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>drugs_yn</t>
+          <t>dx_adhd</t>
         </is>
       </c>
       <c r="B27">
@@ -715,7 +715,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>dx_adhd</t>
+          <t>dx_bi</t>
         </is>
       </c>
       <c r="B28">
@@ -728,7 +728,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>dx_bi</t>
+          <t>dx_dep</t>
         </is>
       </c>
       <c r="B29">
@@ -741,7 +741,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>dx_dep</t>
+          <t>dx_pers</t>
         </is>
       </c>
       <c r="B30">
@@ -754,7 +754,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>dx_pers</t>
+          <t>dx_tr</t>
         </is>
       </c>
       <c r="B31">
@@ -767,7 +767,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>dx_tr</t>
+          <t>ed_any</t>
         </is>
       </c>
       <c r="B32">
@@ -780,7 +780,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ed_any</t>
+          <t>env_mh</t>
         </is>
       </c>
       <c r="B33">
@@ -793,7 +793,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>env_mh</t>
+          <t>fincur</t>
         </is>
       </c>
       <c r="B34">
@@ -806,7 +806,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>fincur</t>
+          <t>finpast</t>
         </is>
       </c>
       <c r="B35">
@@ -819,7 +819,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>finpast</t>
+          <t>flourish</t>
         </is>
       </c>
       <c r="B36">
@@ -832,7 +832,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>flourish</t>
+          <t>gad7_impa</t>
         </is>
       </c>
       <c r="B37">
@@ -845,7 +845,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>gad7_impa</t>
+          <t>gender_noncis</t>
         </is>
       </c>
       <c r="B38">
@@ -858,7 +858,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>gender_noncis</t>
+          <t>gpa_sr</t>
         </is>
       </c>
       <c r="B39">
@@ -871,7 +871,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>gpa_sr</t>
+          <t>inf</t>
         </is>
       </c>
       <c r="B40">
@@ -884,7 +884,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>inf</t>
+          <t>ins_cover</t>
         </is>
       </c>
       <c r="B41">
@@ -897,7 +897,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ins_cover</t>
+          <t>international</t>
         </is>
       </c>
       <c r="B42">
@@ -910,7 +910,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>international</t>
+          <t>meds_anx</t>
         </is>
       </c>
       <c r="B43">
@@ -923,7 +923,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>meds_anx</t>
+          <t>meds_count</t>
         </is>
       </c>
       <c r="B44">
@@ -936,7 +936,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>meds_count</t>
+          <t>meds_dep</t>
         </is>
       </c>
       <c r="B45">
@@ -949,7 +949,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>meds_dep</t>
+          <t>meds_mood</t>
         </is>
       </c>
       <c r="B46">
@@ -962,7 +962,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>meds_mood</t>
+          <t>meds_sle</t>
         </is>
       </c>
       <c r="B47">
@@ -975,7 +975,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>meds_sle</t>
+          <t>meds_sti</t>
         </is>
       </c>
       <c r="B48">
@@ -988,7 +988,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>meds_sti</t>
+          <t>military</t>
         </is>
       </c>
       <c r="B49">
@@ -1001,7 +1001,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>military</t>
+          <t>percneed_cur</t>
         </is>
       </c>
       <c r="B50">
@@ -1014,7 +1014,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>percneed_cur</t>
+          <t>persist</t>
         </is>
       </c>
       <c r="B51">
@@ -1027,7 +1027,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>persist</t>
+          <t>psyhx</t>
         </is>
       </c>
       <c r="B52">
@@ -1040,7 +1040,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>psyhx</t>
+          <t>race</t>
         </is>
       </c>
       <c r="B53">
@@ -1053,7 +1053,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>race</t>
+          <t>religios</t>
         </is>
       </c>
       <c r="B54">
@@ -1066,7 +1066,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>religios</t>
+          <t>residenc</t>
         </is>
       </c>
       <c r="B55">
@@ -1079,7 +1079,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>residenc</t>
+          <t>satisfied_overall</t>
         </is>
       </c>
       <c r="B56">
@@ -1092,7 +1092,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>satisfied_overall</t>
+          <t>school2_type</t>
         </is>
       </c>
       <c r="B57">
@@ -1105,7 +1105,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>school2_type</t>
+          <t>sexual</t>
         </is>
       </c>
       <c r="B58">
@@ -1118,7 +1118,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>sexual</t>
+          <t>sib_freq</t>
         </is>
       </c>
       <c r="B59">
@@ -1131,7 +1131,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>sib_freq</t>
+          <t>stig_pcv_2</t>
         </is>
       </c>
       <c r="B60">
@@ -1144,7 +1144,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>stig_pcv_2</t>
+          <t>stig_pcv_3</t>
         </is>
       </c>
       <c r="B61">
@@ -1157,7 +1157,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>stig_pcv_3</t>
+          <t>talk</t>
         </is>
       </c>
       <c r="B62">
@@ -1170,7 +1170,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>talk</t>
+          <t>ther_vis</t>
         </is>
       </c>
       <c r="B63">
@@ -1178,19 +1178,6 @@
       </c>
       <c r="C63">
         <v>0.7935120690410479</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>ther_vis</t>
-        </is>
-      </c>
-      <c r="B64">
-        <v>36303</v>
-      </c>
-      <c r="C64">
-        <v>0.7951767643579971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
for loops in for brs, aaq, flourish. tried to get t-sne working on train and test overall data (unknown need)
</commit_message>
<xml_diff>
--- a/overall_missing.xlsx
+++ b/overall_missing.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,7 +377,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>aaq_yn</t>
+          <t>aaq_dum</t>
         </is>
       </c>
       <c r="B2">
@@ -442,7 +442,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>anx_mod</t>
+          <t>anx_score</t>
         </is>
       </c>
       <c r="B7">
@@ -455,7 +455,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>anx_sev</t>
+          <t>assault_emo</t>
         </is>
       </c>
       <c r="B8">
@@ -468,7 +468,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>assault_emo</t>
+          <t>assault_phys</t>
         </is>
       </c>
       <c r="B9">
@@ -481,7 +481,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>assault_phys</t>
+          <t>assault_sex</t>
         </is>
       </c>
       <c r="B10">
@@ -494,7 +494,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>assault_sex</t>
+          <t>audit_tot</t>
         </is>
       </c>
       <c r="B11">
@@ -507,7 +507,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>audit_tot</t>
+          <t>belong1</t>
         </is>
       </c>
       <c r="B12">
@@ -520,7 +520,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>belong1</t>
+          <t>belong2</t>
         </is>
       </c>
       <c r="B13">
@@ -533,7 +533,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>belong2</t>
+          <t>belong8</t>
         </is>
       </c>
       <c r="B14">
@@ -546,7 +546,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>belong8</t>
+          <t>belong9</t>
         </is>
       </c>
       <c r="B15">
@@ -559,7 +559,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>belong9</t>
+          <t>binge_fr</t>
         </is>
       </c>
       <c r="B16">
@@ -572,7 +572,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>binge_fr</t>
+          <t>body_sr</t>
         </is>
       </c>
       <c r="B17">
@@ -585,7 +585,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>body_sr</t>
+          <t>brs_dum</t>
         </is>
       </c>
       <c r="B18">
@@ -598,7 +598,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BRS_tot</t>
+          <t>dep_impa</t>
         </is>
       </c>
       <c r="B19">
@@ -611,7 +611,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>dep_impa</t>
+          <t>dep_secret</t>
         </is>
       </c>
       <c r="B20">
@@ -624,7 +624,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>dep_secret</t>
+          <t>deprawsc</t>
         </is>
       </c>
       <c r="B21">
@@ -637,7 +637,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>deprawsc</t>
+          <t>discrim</t>
         </is>
       </c>
       <c r="B22">
@@ -650,7 +650,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>discrim</t>
+          <t>divers</t>
         </is>
       </c>
       <c r="B23">
@@ -663,7 +663,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>divers</t>
+          <t>drug_mar</t>
         </is>
       </c>
       <c r="B24">
@@ -676,7 +676,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>drug_mar</t>
+          <t>drugs_yn</t>
         </is>
       </c>
       <c r="B25">
@@ -689,7 +689,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>drugs_yn</t>
+          <t>dx_adhd</t>
         </is>
       </c>
       <c r="B26">
@@ -702,7 +702,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>dx_adhd</t>
+          <t>dx_bi</t>
         </is>
       </c>
       <c r="B27">
@@ -715,7 +715,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>dx_bi</t>
+          <t>dx_dep</t>
         </is>
       </c>
       <c r="B28">
@@ -728,7 +728,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>dx_dep</t>
+          <t>dx_pers</t>
         </is>
       </c>
       <c r="B29">
@@ -741,7 +741,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>dx_pers</t>
+          <t>dx_tr</t>
         </is>
       </c>
       <c r="B30">
@@ -754,7 +754,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>dx_tr</t>
+          <t>ed_any</t>
         </is>
       </c>
       <c r="B31">
@@ -767,7 +767,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ed_any</t>
+          <t>env_mh</t>
         </is>
       </c>
       <c r="B32">
@@ -780,7 +780,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>env_mh</t>
+          <t>fincur</t>
         </is>
       </c>
       <c r="B33">
@@ -793,7 +793,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>fincur</t>
+          <t>finpast</t>
         </is>
       </c>
       <c r="B34">
@@ -806,7 +806,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>finpast</t>
+          <t>flourish_dum</t>
         </is>
       </c>
       <c r="B35">
@@ -819,7 +819,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>flourish</t>
+          <t>gad7_impa</t>
         </is>
       </c>
       <c r="B36">
@@ -832,7 +832,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>gad7_impa</t>
+          <t>gender_noncis</t>
         </is>
       </c>
       <c r="B37">
@@ -845,7 +845,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>gender_noncis</t>
+          <t>gpa_sr</t>
         </is>
       </c>
       <c r="B38">
@@ -858,7 +858,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>gpa_sr</t>
+          <t>inf</t>
         </is>
       </c>
       <c r="B39">
@@ -871,7 +871,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>inf</t>
+          <t>ins_cover</t>
         </is>
       </c>
       <c r="B40">
@@ -884,7 +884,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ins_cover</t>
+          <t>international</t>
         </is>
       </c>
       <c r="B41">
@@ -897,7 +897,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>international</t>
+          <t>meds_anx</t>
         </is>
       </c>
       <c r="B42">
@@ -910,7 +910,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>meds_anx</t>
+          <t>meds_count</t>
         </is>
       </c>
       <c r="B43">
@@ -923,7 +923,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>meds_count</t>
+          <t>meds_dep</t>
         </is>
       </c>
       <c r="B44">
@@ -936,7 +936,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>meds_dep</t>
+          <t>meds_mood</t>
         </is>
       </c>
       <c r="B45">
@@ -949,7 +949,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>meds_mood</t>
+          <t>meds_sle</t>
         </is>
       </c>
       <c r="B46">
@@ -962,7 +962,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>meds_sle</t>
+          <t>meds_sti</t>
         </is>
       </c>
       <c r="B47">
@@ -975,7 +975,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>meds_sti</t>
+          <t>military</t>
         </is>
       </c>
       <c r="B48">
@@ -988,7 +988,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>military</t>
+          <t>percneed_cur</t>
         </is>
       </c>
       <c r="B49">
@@ -1001,7 +1001,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>percneed_cur</t>
+          <t>persist</t>
         </is>
       </c>
       <c r="B50">
@@ -1014,7 +1014,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>persist</t>
+          <t>psyhx</t>
         </is>
       </c>
       <c r="B51">
@@ -1027,7 +1027,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>psyhx</t>
+          <t>race</t>
         </is>
       </c>
       <c r="B52">
@@ -1040,7 +1040,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>race</t>
+          <t>religios</t>
         </is>
       </c>
       <c r="B53">
@@ -1053,7 +1053,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>religios</t>
+          <t>residenc</t>
         </is>
       </c>
       <c r="B54">
@@ -1066,7 +1066,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>residenc</t>
+          <t>satisfied_overall</t>
         </is>
       </c>
       <c r="B55">
@@ -1079,7 +1079,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>satisfied_overall</t>
+          <t>school2_type</t>
         </is>
       </c>
       <c r="B56">
@@ -1092,7 +1092,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>school2_type</t>
+          <t>sexual</t>
         </is>
       </c>
       <c r="B57">
@@ -1105,7 +1105,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>sexual</t>
+          <t>sib_freq</t>
         </is>
       </c>
       <c r="B58">
@@ -1118,7 +1118,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>sib_freq</t>
+          <t>stig_pcv_2</t>
         </is>
       </c>
       <c r="B59">
@@ -1131,7 +1131,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>stig_pcv_2</t>
+          <t>stig_pcv_3</t>
         </is>
       </c>
       <c r="B60">
@@ -1144,7 +1144,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>stig_pcv_3</t>
+          <t>talk</t>
         </is>
       </c>
       <c r="B61">
@@ -1157,7 +1157,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>talk</t>
+          <t>ther_vis</t>
         </is>
       </c>
       <c r="B62">
@@ -1165,19 +1165,6 @@
       </c>
       <c r="C62">
         <v>0.7956586498444824</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>ther_vis</t>
-        </is>
-      </c>
-      <c r="B63">
-        <v>36227</v>
-      </c>
-      <c r="C63">
-        <v>0.7935120690410479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
playing with SEM code, specifying model
</commit_message>
<xml_diff>
--- a/overall_missing.xlsx
+++ b/overall_missing.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -394,7 +394,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -407,10 +407,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>45641</v>
+        <v>45676</v>
       </c>
       <c r="C4">
-        <v>0.9997152494852587</v>
+        <v>0.9997154676180262</v>
       </c>
     </row>
     <row r="5">
@@ -420,7 +420,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -446,10 +446,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>45595</v>
+        <v>45627</v>
       </c>
       <c r="C7">
-        <v>0.9987076707407894</v>
+        <v>0.9986429994090481</v>
       </c>
     </row>
     <row r="8">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -475,7 +475,7 @@
         <v>297</v>
       </c>
       <c r="C9">
-        <v>0.006505454067551584</v>
+        <v>0.006500470572785572</v>
       </c>
     </row>
     <row r="10">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>45654</v>
+        <v>45689</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -592,7 +592,7 @@
         <v>1281</v>
       </c>
       <c r="C18">
-        <v>0.0280588776448942</v>
+        <v>0.02803738317757009</v>
       </c>
     </row>
     <row r="19">
@@ -602,10 +602,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>45603</v>
+        <v>45638</v>
       </c>
       <c r="C19">
-        <v>0.9988829018267841</v>
+        <v>0.9988837575784105</v>
       </c>
     </row>
     <row r="20">
@@ -615,10 +615,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>2911</v>
+        <v>2915</v>
       </c>
       <c r="C20">
-        <v>0.06376221141630525</v>
+        <v>0.06380091488104357</v>
       </c>
     </row>
     <row r="21">
@@ -628,10 +628,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C21">
-        <v>0.01471941122355106</v>
+        <v>0.0147300225437195</v>
       </c>
     </row>
     <row r="22">
@@ -641,10 +641,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>7210</v>
+        <v>7218</v>
       </c>
       <c r="C22">
-        <v>0.1579270162526832</v>
+        <v>0.1579811333143645</v>
       </c>
     </row>
     <row r="23">
@@ -654,10 +654,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>5237</v>
+        <v>5240</v>
       </c>
       <c r="C23">
-        <v>0.1147106496692513</v>
+        <v>0.1146884370417387</v>
       </c>
     </row>
     <row r="24">
@@ -670,7 +670,7 @@
         <v>1016</v>
       </c>
       <c r="C24">
-        <v>0.02225434792132124</v>
+        <v>0.02223730000656613</v>
       </c>
     </row>
     <row r="25">
@@ -680,10 +680,10 @@
         </is>
       </c>
       <c r="B25">
-        <v>32969</v>
+        <v>32992</v>
       </c>
       <c r="C25">
-        <v>0.7221492092697245</v>
+        <v>0.7220994112368404</v>
       </c>
     </row>
     <row r="26">
@@ -693,10 +693,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C26">
-        <v>0.01537652779603102</v>
+        <v>0.01538663573288976</v>
       </c>
     </row>
     <row r="27">
@@ -719,10 +719,10 @@
         </is>
       </c>
       <c r="B28">
-        <v>45621</v>
+        <v>45656</v>
       </c>
       <c r="C28">
-        <v>0.9992771717702721</v>
+        <v>0.9992777254919127</v>
       </c>
     </row>
     <row r="29">
@@ -732,10 +732,10 @@
         </is>
       </c>
       <c r="B29">
-        <v>45633</v>
+        <v>45659</v>
       </c>
       <c r="C29">
-        <v>0.999540018399264</v>
+        <v>0.9993433868108298</v>
       </c>
     </row>
     <row r="30">
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>45624</v>
+        <v>45650</v>
       </c>
       <c r="C30">
-        <v>0.9993428834275201</v>
+        <v>0.9991464028540786</v>
       </c>
     </row>
     <row r="31">
@@ -774,7 +774,7 @@
         <v>45654</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0.9992339512793014</v>
       </c>
     </row>
     <row r="33">
@@ -784,10 +784,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>36021</v>
+        <v>36040</v>
       </c>
       <c r="C33">
-        <v>0.7889998685766855</v>
+        <v>0.7888113112565388</v>
       </c>
     </row>
     <row r="34">
@@ -797,10 +797,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>44458</v>
+        <v>44490</v>
       </c>
       <c r="C34">
-        <v>0.973802952643799</v>
+        <v>0.9737573595394953</v>
       </c>
     </row>
     <row r="35">
@@ -810,10 +810,10 @@
         </is>
       </c>
       <c r="B35">
-        <v>45595</v>
+        <v>45628</v>
       </c>
       <c r="C35">
-        <v>0.9987076707407894</v>
+        <v>0.9986648865153538</v>
       </c>
     </row>
     <row r="36">
@@ -823,10 +823,10 @@
         </is>
       </c>
       <c r="B36">
-        <v>45268</v>
+        <v>45298</v>
       </c>
       <c r="C36">
-        <v>0.9915451001007579</v>
+        <v>0.991442141434481</v>
       </c>
     </row>
     <row r="37">
@@ -836,10 +836,10 @@
         </is>
       </c>
       <c r="B37">
-        <v>45537</v>
+        <v>45570</v>
       </c>
       <c r="C37">
-        <v>0.9974372453673281</v>
+        <v>0.9973954343496246</v>
       </c>
     </row>
     <row r="38">
@@ -849,10 +849,10 @@
         </is>
       </c>
       <c r="B38">
-        <v>45372</v>
+        <v>45405</v>
       </c>
       <c r="C38">
-        <v>0.9938231042186884</v>
+        <v>0.9937840618091882</v>
       </c>
     </row>
     <row r="39">
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>45642</v>
+        <v>45677</v>
       </c>
       <c r="C39">
-        <v>0.999737153371008</v>
+        <v>0.9997373547243319</v>
       </c>
     </row>
     <row r="40">
@@ -875,10 +875,10 @@
         </is>
       </c>
       <c r="B40">
-        <v>45624</v>
+        <v>45659</v>
       </c>
       <c r="C40">
-        <v>0.9993428834275201</v>
+        <v>0.9993433868108298</v>
       </c>
     </row>
     <row r="41">
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="B41">
-        <v>45619</v>
+        <v>45654</v>
       </c>
       <c r="C41">
-        <v>0.9992333639987734</v>
+        <v>0.9992339512793014</v>
       </c>
     </row>
     <row r="42">
@@ -901,10 +901,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="C42">
-        <v>0.02674464449993429</v>
+        <v>0.02674604390553525</v>
       </c>
     </row>
     <row r="43">
@@ -917,7 +917,7 @@
         <v>78</v>
       </c>
       <c r="C43">
-        <v>0.001708503088447891</v>
+        <v>0.001707194291842675</v>
       </c>
     </row>
     <row r="44">
@@ -930,7 +930,7 @@
         <v>843</v>
       </c>
       <c r="C44">
-        <v>0.01846497568668682</v>
+        <v>0.0184508306156843</v>
       </c>
     </row>
     <row r="45">
@@ -943,7 +943,7 @@
         <v>121</v>
       </c>
       <c r="C45">
-        <v>0.002650370175669164</v>
+        <v>0.002648339862986715</v>
       </c>
     </row>
     <row r="46">
@@ -956,7 +956,7 @@
         <v>300</v>
       </c>
       <c r="C46">
-        <v>0.006571165724799579</v>
+        <v>0.006566131891702598</v>
       </c>
     </row>
     <row r="47">
@@ -969,7 +969,7 @@
         <v>575</v>
       </c>
       <c r="C47">
-        <v>0.01259473430586586</v>
+        <v>0.01258508612576331</v>
       </c>
     </row>
     <row r="48">
@@ -982,7 +982,7 @@
         <v>1358</v>
       </c>
       <c r="C48">
-        <v>0.02974547684759276</v>
+        <v>0.02972269036310709</v>
       </c>
     </row>
     <row r="49">
@@ -995,7 +995,7 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>0.00181802251719455</v>
+        <v>0.001816629823371052</v>
       </c>
     </row>
     <row r="50">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C50">
-        <v>0.006571165724799579</v>
+        <v>0.006588018998008273</v>
       </c>
     </row>
     <row r="51">
@@ -1021,7 +1021,7 @@
         <v>288</v>
       </c>
       <c r="C51">
-        <v>0.006308319095807596</v>
+        <v>0.006303486616034494</v>
       </c>
     </row>
     <row r="52">
@@ -1031,10 +1031,10 @@
         </is>
       </c>
       <c r="B52">
-        <v>3384</v>
+        <v>3386</v>
       </c>
       <c r="C52">
-        <v>0.07412274937573926</v>
+        <v>0.07410974195101666</v>
       </c>
     </row>
     <row r="53">
@@ -1044,10 +1044,10 @@
         </is>
       </c>
       <c r="B53">
-        <v>45534</v>
+        <v>45568</v>
       </c>
       <c r="C53">
-        <v>0.9973715337100801</v>
+        <v>0.9973516601370133</v>
       </c>
     </row>
     <row r="54">
@@ -1057,10 +1057,10 @@
         </is>
       </c>
       <c r="B54">
-        <v>45608</v>
+        <v>45642</v>
       </c>
       <c r="C54">
-        <v>0.9989924212555308</v>
+        <v>0.9989713060036333</v>
       </c>
     </row>
     <row r="55">
@@ -1070,10 +1070,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>45619</v>
+        <v>45653</v>
       </c>
       <c r="C55">
-        <v>0.9992333639987734</v>
+        <v>0.9992120641729957</v>
       </c>
     </row>
     <row r="56">
@@ -1083,10 +1083,10 @@
         </is>
       </c>
       <c r="B56">
-        <v>45607</v>
+        <v>45641</v>
       </c>
       <c r="C56">
-        <v>0.9989705173697814</v>
+        <v>0.9989494188973276</v>
       </c>
     </row>
     <row r="57">
@@ -1096,10 +1096,10 @@
         </is>
       </c>
       <c r="B57">
-        <v>45607</v>
+        <v>45641</v>
       </c>
       <c r="C57">
-        <v>0.9989705173697814</v>
+        <v>0.9989494188973276</v>
       </c>
     </row>
     <row r="58">
@@ -1109,10 +1109,10 @@
         </is>
       </c>
       <c r="B58">
-        <v>45598</v>
+        <v>45632</v>
       </c>
       <c r="C58">
-        <v>0.9987733823980374</v>
+        <v>0.9987524349405765</v>
       </c>
     </row>
     <row r="59">
@@ -1122,10 +1122,10 @@
         </is>
       </c>
       <c r="B59">
-        <v>45605</v>
+        <v>45639</v>
       </c>
       <c r="C59">
-        <v>0.9989267095982828</v>
+        <v>0.9989056446847162</v>
       </c>
     </row>
     <row r="60">
@@ -1135,10 +1135,10 @@
         </is>
       </c>
       <c r="B60">
-        <v>45610</v>
+        <v>45644</v>
       </c>
       <c r="C60">
-        <v>0.9990362290270294</v>
+        <v>0.9990150802162446</v>
       </c>
     </row>
     <row r="61">
@@ -1148,10 +1148,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>45343</v>
+        <v>45377</v>
       </c>
       <c r="C61">
-        <v>0.9931878915319577</v>
+        <v>0.9931712228326293</v>
       </c>
     </row>
     <row r="62">
@@ -1161,10 +1161,10 @@
         </is>
       </c>
       <c r="B62">
-        <v>36325</v>
+        <v>36354</v>
       </c>
       <c r="C62">
-        <v>0.7956586498444824</v>
+        <v>0.7956838626365208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stupid SEM. Still revising, updated save. Was able to output results_sem to Mplus, but MP is killing my will to live.
Former-commit-id: a35230b6e666c56d916083418cbe3a2d81f74843
</commit_message>
<xml_diff>
--- a/overall_missing.xlsx
+++ b/overall_missing.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -394,7 +394,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -407,10 +407,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>45676</v>
+        <v>45641</v>
       </c>
       <c r="C4">
-        <v>0.9997154676180262</v>
+        <v>0.9997152494852587</v>
       </c>
     </row>
     <row r="5">
@@ -420,7 +420,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -446,10 +446,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>45627</v>
+        <v>45595</v>
       </c>
       <c r="C7">
-        <v>0.9986429994090481</v>
+        <v>0.9987076707407894</v>
       </c>
     </row>
     <row r="8">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -475,7 +475,7 @@
         <v>297</v>
       </c>
       <c r="C9">
-        <v>0.006500470572785572</v>
+        <v>0.006505454067551584</v>
       </c>
     </row>
     <row r="10">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>45689</v>
+        <v>45654</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -592,7 +592,7 @@
         <v>1281</v>
       </c>
       <c r="C18">
-        <v>0.02803738317757009</v>
+        <v>0.0280588776448942</v>
       </c>
     </row>
     <row r="19">
@@ -602,10 +602,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>45638</v>
+        <v>45603</v>
       </c>
       <c r="C19">
-        <v>0.9988837575784105</v>
+        <v>0.9988829018267841</v>
       </c>
     </row>
     <row r="20">
@@ -615,10 +615,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>2915</v>
+        <v>2911</v>
       </c>
       <c r="C20">
-        <v>0.06380091488104357</v>
+        <v>0.06376221141630525</v>
       </c>
     </row>
     <row r="21">
@@ -628,10 +628,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C21">
-        <v>0.0147300225437195</v>
+        <v>0.01471941122355106</v>
       </c>
     </row>
     <row r="22">
@@ -641,10 +641,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>7218</v>
+        <v>7210</v>
       </c>
       <c r="C22">
-        <v>0.1579811333143645</v>
+        <v>0.1579270162526832</v>
       </c>
     </row>
     <row r="23">
@@ -654,10 +654,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>5240</v>
+        <v>5237</v>
       </c>
       <c r="C23">
-        <v>0.1146884370417387</v>
+        <v>0.1147106496692513</v>
       </c>
     </row>
     <row r="24">
@@ -670,7 +670,7 @@
         <v>1016</v>
       </c>
       <c r="C24">
-        <v>0.02223730000656613</v>
+        <v>0.02225434792132124</v>
       </c>
     </row>
     <row r="25">
@@ -680,10 +680,10 @@
         </is>
       </c>
       <c r="B25">
-        <v>32992</v>
+        <v>32969</v>
       </c>
       <c r="C25">
-        <v>0.7220994112368404</v>
+        <v>0.7221492092697245</v>
       </c>
     </row>
     <row r="26">
@@ -693,10 +693,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C26">
-        <v>0.01538663573288976</v>
+        <v>0.01537652779603102</v>
       </c>
     </row>
     <row r="27">
@@ -719,10 +719,10 @@
         </is>
       </c>
       <c r="B28">
-        <v>45656</v>
+        <v>45621</v>
       </c>
       <c r="C28">
-        <v>0.9992777254919127</v>
+        <v>0.9992771717702721</v>
       </c>
     </row>
     <row r="29">
@@ -732,10 +732,10 @@
         </is>
       </c>
       <c r="B29">
-        <v>45659</v>
+        <v>45633</v>
       </c>
       <c r="C29">
-        <v>0.9993433868108298</v>
+        <v>0.999540018399264</v>
       </c>
     </row>
     <row r="30">
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>45650</v>
+        <v>45624</v>
       </c>
       <c r="C30">
-        <v>0.9991464028540786</v>
+        <v>0.9993428834275201</v>
       </c>
     </row>
     <row r="31">
@@ -774,7 +774,7 @@
         <v>45654</v>
       </c>
       <c r="C32">
-        <v>0.9992339512793014</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -784,10 +784,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>36040</v>
+        <v>36021</v>
       </c>
       <c r="C33">
-        <v>0.7888113112565388</v>
+        <v>0.7889998685766855</v>
       </c>
     </row>
     <row r="34">
@@ -797,10 +797,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>44490</v>
+        <v>44458</v>
       </c>
       <c r="C34">
-        <v>0.9737573595394953</v>
+        <v>0.973802952643799</v>
       </c>
     </row>
     <row r="35">
@@ -810,10 +810,10 @@
         </is>
       </c>
       <c r="B35">
-        <v>45628</v>
+        <v>45595</v>
       </c>
       <c r="C35">
-        <v>0.9986648865153538</v>
+        <v>0.9987076707407894</v>
       </c>
     </row>
     <row r="36">
@@ -823,10 +823,10 @@
         </is>
       </c>
       <c r="B36">
-        <v>45298</v>
+        <v>45268</v>
       </c>
       <c r="C36">
-        <v>0.991442141434481</v>
+        <v>0.9915451001007579</v>
       </c>
     </row>
     <row r="37">
@@ -836,10 +836,10 @@
         </is>
       </c>
       <c r="B37">
-        <v>45570</v>
+        <v>45537</v>
       </c>
       <c r="C37">
-        <v>0.9973954343496246</v>
+        <v>0.9974372453673281</v>
       </c>
     </row>
     <row r="38">
@@ -849,10 +849,10 @@
         </is>
       </c>
       <c r="B38">
-        <v>45405</v>
+        <v>45372</v>
       </c>
       <c r="C38">
-        <v>0.9937840618091882</v>
+        <v>0.9938231042186884</v>
       </c>
     </row>
     <row r="39">
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>45677</v>
+        <v>45642</v>
       </c>
       <c r="C39">
-        <v>0.9997373547243319</v>
+        <v>0.999737153371008</v>
       </c>
     </row>
     <row r="40">
@@ -875,10 +875,10 @@
         </is>
       </c>
       <c r="B40">
-        <v>45659</v>
+        <v>45624</v>
       </c>
       <c r="C40">
-        <v>0.9993433868108298</v>
+        <v>0.9993428834275201</v>
       </c>
     </row>
     <row r="41">
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="B41">
-        <v>45654</v>
+        <v>45619</v>
       </c>
       <c r="C41">
-        <v>0.9992339512793014</v>
+        <v>0.9992333639987734</v>
       </c>
     </row>
     <row r="42">
@@ -901,10 +901,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C42">
-        <v>0.02674604390553525</v>
+        <v>0.02674464449993429</v>
       </c>
     </row>
     <row r="43">
@@ -917,7 +917,7 @@
         <v>78</v>
       </c>
       <c r="C43">
-        <v>0.001707194291842675</v>
+        <v>0.001708503088447891</v>
       </c>
     </row>
     <row r="44">
@@ -930,7 +930,7 @@
         <v>843</v>
       </c>
       <c r="C44">
-        <v>0.0184508306156843</v>
+        <v>0.01846497568668682</v>
       </c>
     </row>
     <row r="45">
@@ -943,7 +943,7 @@
         <v>121</v>
       </c>
       <c r="C45">
-        <v>0.002648339862986715</v>
+        <v>0.002650370175669164</v>
       </c>
     </row>
     <row r="46">
@@ -956,7 +956,7 @@
         <v>300</v>
       </c>
       <c r="C46">
-        <v>0.006566131891702598</v>
+        <v>0.006571165724799579</v>
       </c>
     </row>
     <row r="47">
@@ -969,7 +969,7 @@
         <v>575</v>
       </c>
       <c r="C47">
-        <v>0.01258508612576331</v>
+        <v>0.01259473430586586</v>
       </c>
     </row>
     <row r="48">
@@ -982,7 +982,7 @@
         <v>1358</v>
       </c>
       <c r="C48">
-        <v>0.02972269036310709</v>
+        <v>0.02974547684759276</v>
       </c>
     </row>
     <row r="49">
@@ -995,7 +995,7 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>0.001816629823371052</v>
+        <v>0.00181802251719455</v>
       </c>
     </row>
     <row r="50">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C50">
-        <v>0.006588018998008273</v>
+        <v>0.006571165724799579</v>
       </c>
     </row>
     <row r="51">
@@ -1021,7 +1021,7 @@
         <v>288</v>
       </c>
       <c r="C51">
-        <v>0.006303486616034494</v>
+        <v>0.006308319095807596</v>
       </c>
     </row>
     <row r="52">
@@ -1031,10 +1031,10 @@
         </is>
       </c>
       <c r="B52">
-        <v>3386</v>
+        <v>3384</v>
       </c>
       <c r="C52">
-        <v>0.07410974195101666</v>
+        <v>0.07412274937573926</v>
       </c>
     </row>
     <row r="53">
@@ -1044,10 +1044,10 @@
         </is>
       </c>
       <c r="B53">
-        <v>45568</v>
+        <v>45534</v>
       </c>
       <c r="C53">
-        <v>0.9973516601370133</v>
+        <v>0.9973715337100801</v>
       </c>
     </row>
     <row r="54">
@@ -1057,10 +1057,10 @@
         </is>
       </c>
       <c r="B54">
-        <v>45642</v>
+        <v>45608</v>
       </c>
       <c r="C54">
-        <v>0.9989713060036333</v>
+        <v>0.9989924212555308</v>
       </c>
     </row>
     <row r="55">
@@ -1070,10 +1070,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>45653</v>
+        <v>45619</v>
       </c>
       <c r="C55">
-        <v>0.9992120641729957</v>
+        <v>0.9992333639987734</v>
       </c>
     </row>
     <row r="56">
@@ -1083,10 +1083,10 @@
         </is>
       </c>
       <c r="B56">
-        <v>45641</v>
+        <v>45607</v>
       </c>
       <c r="C56">
-        <v>0.9989494188973276</v>
+        <v>0.9989705173697814</v>
       </c>
     </row>
     <row r="57">
@@ -1096,10 +1096,10 @@
         </is>
       </c>
       <c r="B57">
-        <v>45641</v>
+        <v>45607</v>
       </c>
       <c r="C57">
-        <v>0.9989494188973276</v>
+        <v>0.9989705173697814</v>
       </c>
     </row>
     <row r="58">
@@ -1109,10 +1109,10 @@
         </is>
       </c>
       <c r="B58">
-        <v>45632</v>
+        <v>45598</v>
       </c>
       <c r="C58">
-        <v>0.9987524349405765</v>
+        <v>0.9987733823980374</v>
       </c>
     </row>
     <row r="59">
@@ -1122,10 +1122,10 @@
         </is>
       </c>
       <c r="B59">
-        <v>45639</v>
+        <v>45605</v>
       </c>
       <c r="C59">
-        <v>0.9989056446847162</v>
+        <v>0.9989267095982828</v>
       </c>
     </row>
     <row r="60">
@@ -1135,10 +1135,10 @@
         </is>
       </c>
       <c r="B60">
-        <v>45644</v>
+        <v>45610</v>
       </c>
       <c r="C60">
-        <v>0.9990150802162446</v>
+        <v>0.9990362290270294</v>
       </c>
     </row>
     <row r="61">
@@ -1148,10 +1148,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>45377</v>
+        <v>45343</v>
       </c>
       <c r="C61">
-        <v>0.9931712228326293</v>
+        <v>0.9931878915319577</v>
       </c>
     </row>
     <row r="62">
@@ -1161,10 +1161,10 @@
         </is>
       </c>
       <c r="B62">
-        <v>36354</v>
+        <v>36325</v>
       </c>
       <c r="C62">
-        <v>0.7956838626365208</v>
+        <v>0.7956586498444824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved around specification for train and test data.
Former-commit-id: aa1d1dc42465541d9aebb3262b4b0452c5e0593e
</commit_message>
<xml_diff>
--- a/overall_missing.xlsx
+++ b/overall_missing.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,7 +390,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>abuse_year</t>
+          <t>aca_impa</t>
         </is>
       </c>
       <c r="B3">
@@ -403,7 +403,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>aca_impa</t>
+          <t>activ_yn</t>
         </is>
       </c>
       <c r="B4">
@@ -416,7 +416,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>activ_yn</t>
+          <t>age</t>
         </is>
       </c>
       <c r="B5">
@@ -429,7 +429,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>anx_score</t>
         </is>
       </c>
       <c r="B6">
@@ -442,7 +442,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>anx_score</t>
+          <t>assault_sex</t>
         </is>
       </c>
       <c r="B7">
@@ -455,7 +455,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>assault_emo</t>
+          <t>belong1</t>
         </is>
       </c>
       <c r="B8">
@@ -468,7 +468,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>assault_phys</t>
+          <t>binge_fr</t>
         </is>
       </c>
       <c r="B9">
@@ -481,7 +481,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>assault_sex</t>
+          <t>brs_dum</t>
         </is>
       </c>
       <c r="B10">
@@ -494,7 +494,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>audit_tot</t>
+          <t>dep_impa</t>
         </is>
       </c>
       <c r="B11">
@@ -507,7 +507,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>belong1</t>
+          <t>dep_secret</t>
         </is>
       </c>
       <c r="B12">
@@ -520,7 +520,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>belong2</t>
+          <t>deprawsc</t>
         </is>
       </c>
       <c r="B13">
@@ -533,7 +533,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>belong8</t>
+          <t>discrim</t>
         </is>
       </c>
       <c r="B14">
@@ -546,7 +546,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>belong9</t>
+          <t>divers</t>
         </is>
       </c>
       <c r="B15">
@@ -559,7 +559,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>binge_fr</t>
+          <t>drug_mar</t>
         </is>
       </c>
       <c r="B16">
@@ -572,7 +572,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>body_sr</t>
+          <t>drugs_yn</t>
         </is>
       </c>
       <c r="B17">
@@ -585,7 +585,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>brs_dum</t>
+          <t>dx_adhd</t>
         </is>
       </c>
       <c r="B18">
@@ -598,7 +598,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>dep_impa</t>
+          <t>dx_anx</t>
         </is>
       </c>
       <c r="B19">
@@ -611,7 +611,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>dep_secret</t>
+          <t>dx_bi</t>
         </is>
       </c>
       <c r="B20">
@@ -624,7 +624,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>deprawsc</t>
+          <t>dx_dep</t>
         </is>
       </c>
       <c r="B21">
@@ -637,7 +637,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>discrim</t>
+          <t>dx_pers</t>
         </is>
       </c>
       <c r="B22">
@@ -650,7 +650,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>divers</t>
+          <t>dx_tr</t>
         </is>
       </c>
       <c r="B23">
@@ -663,7 +663,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>drug_mar</t>
+          <t>ed_any</t>
         </is>
       </c>
       <c r="B24">
@@ -676,7 +676,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>drugs_yn</t>
+          <t>fincur</t>
         </is>
       </c>
       <c r="B25">
@@ -689,7 +689,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>dx_adhd</t>
+          <t>flourish_dum</t>
         </is>
       </c>
       <c r="B26">
@@ -702,7 +702,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>dx_bi</t>
+          <t>gad7_impa</t>
         </is>
       </c>
       <c r="B27">
@@ -715,7 +715,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>dx_dep</t>
+          <t>gender_noncis</t>
         </is>
       </c>
       <c r="B28">
@@ -728,7 +728,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>dx_pers</t>
+          <t>gpa_sr</t>
         </is>
       </c>
       <c r="B29">
@@ -741,7 +741,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>dx_tr</t>
+          <t>inf</t>
         </is>
       </c>
       <c r="B30">
@@ -754,7 +754,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ed_any</t>
+          <t>ins_cover</t>
         </is>
       </c>
       <c r="B31">
@@ -767,7 +767,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>env_mh</t>
+          <t>meds_count</t>
         </is>
       </c>
       <c r="B32">
@@ -780,7 +780,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>fincur</t>
+          <t>meds_sti</t>
         </is>
       </c>
       <c r="B33">
@@ -793,7 +793,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>finpast</t>
+          <t>mh_stigma</t>
         </is>
       </c>
       <c r="B34">
@@ -806,7 +806,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>flourish_dum</t>
+          <t>military</t>
         </is>
       </c>
       <c r="B35">
@@ -819,7 +819,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>gad7_impa</t>
+          <t>percneed_cur</t>
         </is>
       </c>
       <c r="B36">
@@ -832,7 +832,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>gender_noncis</t>
+          <t>persist</t>
         </is>
       </c>
       <c r="B37">
@@ -845,7 +845,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>gpa_sr</t>
+          <t>psyhx</t>
         </is>
       </c>
       <c r="B38">
@@ -858,7 +858,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>inf</t>
+          <t>race</t>
         </is>
       </c>
       <c r="B39">
@@ -871,7 +871,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ins_cover</t>
+          <t>religios</t>
         </is>
       </c>
       <c r="B40">
@@ -884,7 +884,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>international</t>
+          <t>satisfied_overall</t>
         </is>
       </c>
       <c r="B41">
@@ -897,7 +897,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>meds_anx</t>
+          <t>school2_type</t>
         </is>
       </c>
       <c r="B42">
@@ -910,7 +910,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>meds_count</t>
+          <t>sexual</t>
         </is>
       </c>
       <c r="B43">
@@ -923,7 +923,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>meds_dep</t>
+          <t>sib_freq</t>
         </is>
       </c>
       <c r="B44">
@@ -936,7 +936,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>meds_mood</t>
+          <t>talk</t>
         </is>
       </c>
       <c r="B45">
@@ -949,7 +949,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>meds_sle</t>
+          <t>trauma_year</t>
         </is>
       </c>
       <c r="B46">
@@ -957,214 +957,6 @@
       </c>
       <c r="C46">
         <v>0.006571165724799579</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>meds_sti</t>
-        </is>
-      </c>
-      <c r="B47">
-        <v>575</v>
-      </c>
-      <c r="C47">
-        <v>0.01259473430586586</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>military</t>
-        </is>
-      </c>
-      <c r="B48">
-        <v>1358</v>
-      </c>
-      <c r="C48">
-        <v>0.02974547684759276</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>percneed_cur</t>
-        </is>
-      </c>
-      <c r="B49">
-        <v>83</v>
-      </c>
-      <c r="C49">
-        <v>0.00181802251719455</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>persist</t>
-        </is>
-      </c>
-      <c r="B50">
-        <v>300</v>
-      </c>
-      <c r="C50">
-        <v>0.006571165724799579</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>psyhx</t>
-        </is>
-      </c>
-      <c r="B51">
-        <v>288</v>
-      </c>
-      <c r="C51">
-        <v>0.006308319095807596</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>race</t>
-        </is>
-      </c>
-      <c r="B52">
-        <v>3384</v>
-      </c>
-      <c r="C52">
-        <v>0.07412274937573926</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>religios</t>
-        </is>
-      </c>
-      <c r="B53">
-        <v>45534</v>
-      </c>
-      <c r="C53">
-        <v>0.9973715337100801</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>residenc</t>
-        </is>
-      </c>
-      <c r="B54">
-        <v>45608</v>
-      </c>
-      <c r="C54">
-        <v>0.9989924212555308</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>satisfied_overall</t>
-        </is>
-      </c>
-      <c r="B55">
-        <v>45619</v>
-      </c>
-      <c r="C55">
-        <v>0.9992333639987734</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>school2_type</t>
-        </is>
-      </c>
-      <c r="B56">
-        <v>45607</v>
-      </c>
-      <c r="C56">
-        <v>0.9989705173697814</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>sexual</t>
-        </is>
-      </c>
-      <c r="B57">
-        <v>45607</v>
-      </c>
-      <c r="C57">
-        <v>0.9989705173697814</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>sib_freq</t>
-        </is>
-      </c>
-      <c r="B58">
-        <v>45598</v>
-      </c>
-      <c r="C58">
-        <v>0.9987733823980374</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>stig_pcv_2</t>
-        </is>
-      </c>
-      <c r="B59">
-        <v>45605</v>
-      </c>
-      <c r="C59">
-        <v>0.9989267095982828</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>stig_pcv_3</t>
-        </is>
-      </c>
-      <c r="B60">
-        <v>45610</v>
-      </c>
-      <c r="C60">
-        <v>0.9990362290270294</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>talk</t>
-        </is>
-      </c>
-      <c r="B61">
-        <v>45343</v>
-      </c>
-      <c r="C61">
-        <v>0.9931878915319577</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>ther_vis</t>
-        </is>
-      </c>
-      <c r="B62">
-        <v>36325</v>
-      </c>
-      <c r="C62">
-        <v>0.7956586498444824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>